<commit_message>
Corrigido Logico e Fisico
</commit_message>
<xml_diff>
--- a/Banco de dados/Modelagem/ModelagemBancodeDados-Fisico.xlsx
+++ b/Banco de dados/Modelagem/ModelagemBancodeDados-Fisico.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renat\Desktop\projeto\Projeto_Inicial-3T\Banco de dados\Modelagem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C347897-28B0-4D38-895A-C661FE982461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1860" yWindow="45" windowWidth="21555" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Usuario</t>
   </si>
@@ -45,15 +54,17 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FFFCE5CD"/>
         <rFont val="Arial"/>
-        <color rgb="FFFCE5CD"/>
       </rPr>
       <t>AD</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <color rgb="FF000000"/>
       </rPr>
       <t>ADM</t>
     </r>
@@ -70,15 +81,17 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FFFCE5CD"/>
         <rFont val="Arial"/>
-        <color rgb="FFFCE5CD"/>
       </rPr>
       <t>AD</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <color rgb="FF000000"/>
       </rPr>
       <t>ADM</t>
     </r>
@@ -95,15 +108,17 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FFFCE5CD"/>
         <rFont val="Arial"/>
-        <color rgb="FFFCE5CD"/>
       </rPr>
       <t>AD</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <color rgb="FF000000"/>
       </rPr>
       <t>ADM</t>
     </r>
@@ -120,15 +135,17 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FFFCE5CD"/>
         <rFont val="Arial"/>
-        <color rgb="FFFCE5CD"/>
       </rPr>
       <t>AD</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <color rgb="FF000000"/>
       </rPr>
       <t>ADM</t>
     </r>
@@ -236,35 +253,45 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFCE5CD"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE69138"/>
-        <bgColor rgb="FFE69138"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -350,101 +377,97 @@
         <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor rgb="FFE69138"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="16" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -634,350 +657,389 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A4:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="23.14"/>
-    <col customWidth="1" min="3" max="3" width="19.43"/>
-    <col customWidth="1" min="4" max="4" width="39.29"/>
-    <col customWidth="1" min="5" max="5" width="22.86"/>
-    <col customWidth="1" min="6" max="6" width="43.57"/>
-    <col customWidth="1" min="8" max="8" width="17.57"/>
-    <col customWidth="1" min="10" max="10" width="17.43"/>
-    <col customWidth="1" min="11" max="11" width="22.14"/>
-    <col customWidth="1" min="12" max="12" width="17.57"/>
-    <col customWidth="1" min="13" max="13" width="18.43"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="E5" s="5" t="s">
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="J4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="E6" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="8" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="E7" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="F7" s="8" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="25">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="K7" s="10" t="s">
+      <c r="J7" s="8">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8">
-      <c r="E8" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="F8" s="8" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D8" s="25">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="K8" s="10" t="s">
+      <c r="J8" s="8">
+        <v>3</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9">
-      <c r="E9" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="F9" s="8" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D9" s="25">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>4</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="G12" s="23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="14" t="s">
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="16" t="s">
+      <c r="N13" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="B14" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="C14" s="19">
-        <v>2.0</v>
-      </c>
-      <c r="D14" s="19" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="H14" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="I14" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="20" t="s">
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+      <c r="J14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="20">
-        <v>1010101.0</v>
-      </c>
-      <c r="L14" s="21" t="s">
+      <c r="K14" s="16">
+        <v>1010101</v>
+      </c>
+      <c r="L14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="20">
-        <v>999.0</v>
-      </c>
-      <c r="N14" s="20" t="s">
+      <c r="M14" s="16">
+        <v>999</v>
+      </c>
+      <c r="N14" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="B15" s="19">
-        <v>2.0</v>
-      </c>
-      <c r="C15" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="D15" s="19" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
+        <v>1</v>
+      </c>
+      <c r="B15" s="15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="15">
+        <v>3</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="H15" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="I15" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="J15" s="20" t="s">
+      <c r="G15" s="16">
+        <v>2</v>
+      </c>
+      <c r="H15" s="16">
+        <v>2</v>
+      </c>
+      <c r="I15" s="16">
+        <v>2</v>
+      </c>
+      <c r="J15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="20">
-        <v>23430.0</v>
-      </c>
-      <c r="L15" s="20" t="s">
+      <c r="K15" s="16">
+        <v>23430</v>
+      </c>
+      <c r="L15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="M15" s="20">
-        <v>728.0</v>
-      </c>
-      <c r="N15" s="20" t="s">
+      <c r="M15" s="16">
+        <v>728</v>
+      </c>
+      <c r="N15" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="B16" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="C16" s="19">
-        <v>4.0</v>
-      </c>
-      <c r="D16" s="19" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="14">
+        <v>1</v>
+      </c>
+      <c r="B16" s="15">
+        <v>3</v>
+      </c>
+      <c r="C16" s="15">
+        <v>4</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="H16" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="I16" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="J16" s="20" t="s">
+      <c r="G16" s="16">
+        <v>3</v>
+      </c>
+      <c r="H16" s="16">
+        <v>3</v>
+      </c>
+      <c r="I16" s="16">
+        <v>3</v>
+      </c>
+      <c r="J16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="20">
-        <v>445432.0</v>
-      </c>
-      <c r="L16" s="20" t="s">
+      <c r="K16" s="16">
+        <v>445432</v>
+      </c>
+      <c r="L16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M16" s="20">
-        <v>188.0</v>
-      </c>
-      <c r="N16" s="20" t="s">
+      <c r="M16" s="16">
+        <v>188</v>
+      </c>
+      <c r="N16" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="22" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="23" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21">
-      <c r="B21" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="C21" s="24" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="19">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="19" t="s">
         <v>55</v>
       </c>
     </row>
@@ -987,8 +1049,9 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="G12:N12"/>
     <mergeCell ref="B19:F19"/>
-    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="D4:H4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>